<commit_message>
add files for trabalho2
</commit_message>
<xml_diff>
--- a/resolucoes/trabalho2/smoke_test.xlsx
+++ b/resolucoes/trabalho2/smoke_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaeltheodoro/Documents/Rodrigo/ED-Caetano/trabalhoII/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaeltheodoro/Documents/Rodrigo/UnBCIC-ED/resolucoes/trabalho2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Tópico</t>
   </si>
@@ -341,6 +341,21 @@
     <t>Popular aleatoriamente características Primordiais</t>
   </si>
   <si>
+    <t>Inserir Primordiais na lista</t>
+  </si>
+  <si>
+    <t>Inserir os 4 Primordiais criados (Tree*) na lista duplamente encadeada respeitando o id do personagem como a posição de alocação na mesma.</t>
+  </si>
+  <si>
+    <t>Imprimindo o Personagem</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>lista_dupla.c</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Implementar a função </t>
     </r>
@@ -371,7 +386,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>define_caracteristicas()</t>
+      <t>definir_caract()</t>
     </r>
     <r>
       <rPr>
@@ -410,7 +425,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>busca_caracteristica()</t>
+      <t>buscar_caract()</t>
     </r>
     <r>
       <rPr>
@@ -422,29 +437,13 @@
       </rPr>
       <t xml:space="preserve"> que retorna o Nodo da característica buscada.</t>
     </r>
-  </si>
-  <si>
-    <t>Inserir Primordiais na lista</t>
-  </si>
-  <si>
-    <t>Inserir os 4 Primordiais criados (Tree*) na lista duplamente encadeada respeitando o id do personagem como a posição de alocação na mesma.</t>
-  </si>
-  <si>
-    <t>Imprimindo o Personagem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -500,10 +499,7 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -519,9 +515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -532,6 +525,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,156 +821,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="144" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="D13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>